<commit_message>
[JH] 4. Data Function
</commit_message>
<xml_diff>
--- a/Chain.of.Heroes/Tools/ExcelParser/Data/SwordWoman.xlsx
+++ b/Chain.of.Heroes/Tools/ExcelParser/Data/SwordWoman.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\junha\OneDrive\문서\GitHub\Chain_Of_Heroes\Chain.of.Heroes\Tools\ExcelParser\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0C78295-0931-4030-968C-8ECB2B1DD631}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86C85869-9DC1-4272-9307-0326E75FFA78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="43200" yWindow="0" windowWidth="14400" windowHeight="16200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -872,8 +872,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
[JH] 5. DataFunction Edit
</commit_message>
<xml_diff>
--- a/Chain.of.Heroes/Tools/ExcelParser/Data/SwordWoman.xlsx
+++ b/Chain.of.Heroes/Tools/ExcelParser/Data/SwordWoman.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\junha\OneDrive\문서\GitHub\Chain_Of_Heroes\Chain.of.Heroes\Tools\ExcelParser\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86C85869-9DC1-4272-9307-0326E75FFA78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE21C78E-07D8-458E-8135-2A94D6C28A67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="43200" yWindow="0" windowWidth="14400" windowHeight="16200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SwordWoman" sheetId="1" r:id="rId1"/>
@@ -872,8 +872,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="K20" sqref="K20"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
[JH] 13. UI&Data Work
</commit_message>
<xml_diff>
--- a/Chain.of.Heroes/Tools/ExcelParser/Data/SwordWoman.xlsx
+++ b/Chain.of.Heroes/Tools/ExcelParser/Data/SwordWoman.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\junha\OneDrive\문서\GitHub\Chain_Of_Heroes\Chain.of.Heroes\Tools\ExcelParser\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HOJIN\Desktop\데이터테이블\캐릭터\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE21C78E-07D8-458E-8135-2A94D6C28A67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCD7CBFD-3CA1-4EA5-B05B-E5B28F02D775}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SwordWoman" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="74">
   <si>
     <t>Int</t>
     <phoneticPr fontId="4" type="noConversion"/>
@@ -148,10 +148,6 @@
   </si>
   <si>
     <t>CharClass</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Knight</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
@@ -872,8 +868,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N44"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="H26" sqref="H26"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -935,7 +931,7 @@
         <v>10</v>
       </c>
       <c r="N1" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
@@ -1026,7 +1022,7 @@
         <v>20</v>
       </c>
       <c r="I4" s="14" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J4" s="14" t="s">
         <v>22</v>
@@ -1049,10 +1045,10 @@
         <v>10010000</v>
       </c>
       <c r="B5" s="17" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C5" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D5" s="17">
         <v>1</v>
@@ -1084,8 +1080,8 @@
       <c r="M5" s="17">
         <v>1.3</v>
       </c>
-      <c r="N5" s="17" t="s">
-        <v>31</v>
+      <c r="N5" s="17">
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.3">
@@ -1093,10 +1089,10 @@
         <v>10010001</v>
       </c>
       <c r="B6" s="17" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C6" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D6" s="17">
         <v>2</v>
@@ -1128,8 +1124,8 @@
       <c r="M6" s="17">
         <v>1.3</v>
       </c>
-      <c r="N6" s="17" t="s">
-        <v>31</v>
+      <c r="N6" s="17">
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.3">
@@ -1137,10 +1133,10 @@
         <v>10010002</v>
       </c>
       <c r="B7" s="17" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C7" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D7" s="17">
         <v>3</v>
@@ -1172,8 +1168,8 @@
       <c r="M7" s="17">
         <v>1.3</v>
       </c>
-      <c r="N7" s="17" t="s">
-        <v>31</v>
+      <c r="N7" s="17">
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.3">
@@ -1181,10 +1177,10 @@
         <v>10010003</v>
       </c>
       <c r="B8" s="17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C8" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D8" s="17">
         <v>4</v>
@@ -1216,8 +1212,8 @@
       <c r="M8" s="17">
         <v>1.3</v>
       </c>
-      <c r="N8" s="17" t="s">
-        <v>31</v>
+      <c r="N8" s="17">
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.3">
@@ -1225,10 +1221,10 @@
         <v>10010004</v>
       </c>
       <c r="B9" s="17" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C9" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D9" s="17">
         <v>5</v>
@@ -1260,8 +1256,8 @@
       <c r="M9" s="17">
         <v>1.3</v>
       </c>
-      <c r="N9" s="17" t="s">
-        <v>31</v>
+      <c r="N9" s="17">
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.3">
@@ -1269,10 +1265,10 @@
         <v>10010005</v>
       </c>
       <c r="B10" s="17" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C10" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D10" s="17">
         <v>6</v>
@@ -1304,8 +1300,8 @@
       <c r="M10" s="17">
         <v>1.3</v>
       </c>
-      <c r="N10" s="17" t="s">
-        <v>31</v>
+      <c r="N10" s="17">
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.3">
@@ -1313,10 +1309,10 @@
         <v>10010006</v>
       </c>
       <c r="B11" s="17" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C11" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D11" s="17">
         <v>7</v>
@@ -1348,8 +1344,8 @@
       <c r="M11" s="17">
         <v>1.3</v>
       </c>
-      <c r="N11" s="17" t="s">
-        <v>31</v>
+      <c r="N11" s="17">
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.3">
@@ -1357,10 +1353,10 @@
         <v>10010007</v>
       </c>
       <c r="B12" s="17" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C12" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D12" s="17">
         <v>8</v>
@@ -1392,8 +1388,8 @@
       <c r="M12" s="17">
         <v>1.3</v>
       </c>
-      <c r="N12" s="17" t="s">
-        <v>31</v>
+      <c r="N12" s="17">
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.3">
@@ -1401,10 +1397,10 @@
         <v>10010008</v>
       </c>
       <c r="B13" s="17" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C13" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D13" s="17">
         <v>9</v>
@@ -1436,8 +1432,8 @@
       <c r="M13" s="17">
         <v>1.3</v>
       </c>
-      <c r="N13" s="17" t="s">
-        <v>31</v>
+      <c r="N13" s="17">
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.3">
@@ -1445,10 +1441,10 @@
         <v>10010009</v>
       </c>
       <c r="B14" s="17" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C14" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D14" s="17">
         <v>10</v>
@@ -1480,8 +1476,8 @@
       <c r="M14" s="17">
         <v>1.3</v>
       </c>
-      <c r="N14" s="17" t="s">
-        <v>31</v>
+      <c r="N14" s="17">
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.3">
@@ -1489,10 +1485,10 @@
         <v>10010010</v>
       </c>
       <c r="B15" s="17" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C15" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D15" s="17">
         <v>11</v>
@@ -1524,8 +1520,8 @@
       <c r="M15" s="17">
         <v>1.3</v>
       </c>
-      <c r="N15" s="17" t="s">
-        <v>31</v>
+      <c r="N15" s="17">
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.3">
@@ -1533,10 +1529,10 @@
         <v>10010011</v>
       </c>
       <c r="B16" s="17" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C16" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D16" s="17">
         <v>12</v>
@@ -1568,8 +1564,8 @@
       <c r="M16" s="17">
         <v>1.3</v>
       </c>
-      <c r="N16" s="17" t="s">
-        <v>31</v>
+      <c r="N16" s="17">
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.3">
@@ -1577,10 +1573,10 @@
         <v>10010012</v>
       </c>
       <c r="B17" s="17" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C17" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D17" s="17">
         <v>13</v>
@@ -1612,8 +1608,8 @@
       <c r="M17" s="17">
         <v>1.3</v>
       </c>
-      <c r="N17" s="17" t="s">
-        <v>31</v>
+      <c r="N17" s="17">
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.3">
@@ -1621,10 +1617,10 @@
         <v>10010013</v>
       </c>
       <c r="B18" s="17" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C18" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D18" s="17">
         <v>14</v>
@@ -1656,8 +1652,8 @@
       <c r="M18" s="17">
         <v>1.3</v>
       </c>
-      <c r="N18" s="17" t="s">
-        <v>31</v>
+      <c r="N18" s="17">
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.3">
@@ -1665,10 +1661,10 @@
         <v>10010014</v>
       </c>
       <c r="B19" s="17" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C19" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D19" s="17">
         <v>15</v>
@@ -1700,8 +1696,8 @@
       <c r="M19" s="17">
         <v>1.3</v>
       </c>
-      <c r="N19" s="17" t="s">
-        <v>31</v>
+      <c r="N19" s="17">
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.3">
@@ -1709,10 +1705,10 @@
         <v>10010015</v>
       </c>
       <c r="B20" s="17" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C20" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D20" s="17">
         <v>16</v>
@@ -1744,8 +1740,8 @@
       <c r="M20" s="17">
         <v>1.3</v>
       </c>
-      <c r="N20" s="17" t="s">
-        <v>31</v>
+      <c r="N20" s="17">
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.3">
@@ -1753,10 +1749,10 @@
         <v>10010016</v>
       </c>
       <c r="B21" s="17" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C21" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D21" s="17">
         <v>17</v>
@@ -1788,8 +1784,8 @@
       <c r="M21" s="17">
         <v>1.3</v>
       </c>
-      <c r="N21" s="17" t="s">
-        <v>31</v>
+      <c r="N21" s="17">
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.3">
@@ -1797,10 +1793,10 @@
         <v>10010017</v>
       </c>
       <c r="B22" s="17" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C22" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D22" s="17">
         <v>18</v>
@@ -1832,8 +1828,8 @@
       <c r="M22" s="17">
         <v>1.3</v>
       </c>
-      <c r="N22" s="17" t="s">
-        <v>31</v>
+      <c r="N22" s="17">
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.3">
@@ -1841,10 +1837,10 @@
         <v>10010018</v>
       </c>
       <c r="B23" s="17" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C23" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D23" s="17">
         <v>19</v>
@@ -1876,8 +1872,8 @@
       <c r="M23" s="17">
         <v>1.3</v>
       </c>
-      <c r="N23" s="17" t="s">
-        <v>31</v>
+      <c r="N23" s="17">
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.3">
@@ -1885,10 +1881,10 @@
         <v>10010019</v>
       </c>
       <c r="B24" s="17" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C24" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D24" s="17">
         <v>20</v>
@@ -1920,8 +1916,8 @@
       <c r="M24" s="17">
         <v>1.3</v>
       </c>
-      <c r="N24" s="17" t="s">
-        <v>31</v>
+      <c r="N24" s="17">
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.3">
@@ -1929,10 +1925,10 @@
         <v>10010020</v>
       </c>
       <c r="B25" s="17" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C25" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D25" s="17">
         <v>21</v>
@@ -1964,8 +1960,8 @@
       <c r="M25" s="17">
         <v>1.3</v>
       </c>
-      <c r="N25" s="17" t="s">
-        <v>31</v>
+      <c r="N25" s="17">
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.3">
@@ -1973,10 +1969,10 @@
         <v>10010021</v>
       </c>
       <c r="B26" s="17" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C26" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D26" s="17">
         <v>22</v>
@@ -2008,8 +2004,8 @@
       <c r="M26" s="17">
         <v>1.3</v>
       </c>
-      <c r="N26" s="17" t="s">
-        <v>31</v>
+      <c r="N26" s="17">
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.3">
@@ -2017,10 +2013,10 @@
         <v>10010022</v>
       </c>
       <c r="B27" s="17" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C27" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D27" s="17">
         <v>23</v>
@@ -2052,8 +2048,8 @@
       <c r="M27" s="17">
         <v>1.3</v>
       </c>
-      <c r="N27" s="17" t="s">
-        <v>31</v>
+      <c r="N27" s="17">
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.3">
@@ -2061,10 +2057,10 @@
         <v>10010023</v>
       </c>
       <c r="B28" s="17" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C28" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D28" s="17">
         <v>24</v>
@@ -2096,8 +2092,8 @@
       <c r="M28" s="17">
         <v>1.3</v>
       </c>
-      <c r="N28" s="17" t="s">
-        <v>31</v>
+      <c r="N28" s="17">
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.3">
@@ -2105,10 +2101,10 @@
         <v>10010024</v>
       </c>
       <c r="B29" s="17" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C29" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D29" s="17">
         <v>25</v>
@@ -2140,8 +2136,8 @@
       <c r="M29" s="17">
         <v>1.3</v>
       </c>
-      <c r="N29" s="17" t="s">
-        <v>31</v>
+      <c r="N29" s="17">
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.3">
@@ -2149,10 +2145,10 @@
         <v>10010025</v>
       </c>
       <c r="B30" s="17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C30" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D30" s="17">
         <v>26</v>
@@ -2184,8 +2180,8 @@
       <c r="M30" s="17">
         <v>1.3</v>
       </c>
-      <c r="N30" s="17" t="s">
-        <v>31</v>
+      <c r="N30" s="17">
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.3">
@@ -2193,10 +2189,10 @@
         <v>10010026</v>
       </c>
       <c r="B31" s="17" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C31" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D31" s="17">
         <v>27</v>
@@ -2228,8 +2224,8 @@
       <c r="M31" s="17">
         <v>1.3</v>
       </c>
-      <c r="N31" s="17" t="s">
-        <v>31</v>
+      <c r="N31" s="17">
+        <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.3">
@@ -2237,10 +2233,10 @@
         <v>10010027</v>
       </c>
       <c r="B32" s="17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C32" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D32" s="17">
         <v>28</v>
@@ -2272,8 +2268,8 @@
       <c r="M32" s="17">
         <v>1.3</v>
       </c>
-      <c r="N32" s="17" t="s">
-        <v>31</v>
+      <c r="N32" s="17">
+        <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.3">
@@ -2281,10 +2277,10 @@
         <v>10010028</v>
       </c>
       <c r="B33" s="17" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C33" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D33" s="17">
         <v>29</v>
@@ -2316,8 +2312,8 @@
       <c r="M33" s="17">
         <v>1.3</v>
       </c>
-      <c r="N33" s="17" t="s">
-        <v>31</v>
+      <c r="N33" s="17">
+        <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.3">
@@ -2325,10 +2321,10 @@
         <v>10010029</v>
       </c>
       <c r="B34" s="17" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C34" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D34" s="17">
         <v>30</v>
@@ -2360,8 +2356,8 @@
       <c r="M34" s="17">
         <v>1.3</v>
       </c>
-      <c r="N34" s="17" t="s">
-        <v>31</v>
+      <c r="N34" s="17">
+        <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.3">
@@ -2369,10 +2365,10 @@
         <v>10010030</v>
       </c>
       <c r="B35" s="17" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C35" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D35" s="17">
         <v>31</v>
@@ -2404,8 +2400,8 @@
       <c r="M35" s="17">
         <v>1.3</v>
       </c>
-      <c r="N35" s="17" t="s">
-        <v>31</v>
+      <c r="N35" s="17">
+        <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.3">
@@ -2413,10 +2409,10 @@
         <v>10010031</v>
       </c>
       <c r="B36" s="17" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C36" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D36" s="17">
         <v>32</v>
@@ -2448,8 +2444,8 @@
       <c r="M36" s="17">
         <v>1.3</v>
       </c>
-      <c r="N36" s="17" t="s">
-        <v>31</v>
+      <c r="N36" s="17">
+        <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.3">
@@ -2457,10 +2453,10 @@
         <v>10010032</v>
       </c>
       <c r="B37" s="17" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C37" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D37" s="17">
         <v>33</v>
@@ -2492,8 +2488,8 @@
       <c r="M37" s="17">
         <v>1.3</v>
       </c>
-      <c r="N37" s="17" t="s">
-        <v>31</v>
+      <c r="N37" s="17">
+        <v>0</v>
       </c>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.3">
@@ -2501,10 +2497,10 @@
         <v>10010033</v>
       </c>
       <c r="B38" s="17" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C38" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D38" s="17">
         <v>34</v>
@@ -2536,8 +2532,8 @@
       <c r="M38" s="17">
         <v>1.3</v>
       </c>
-      <c r="N38" s="17" t="s">
-        <v>31</v>
+      <c r="N38" s="17">
+        <v>0</v>
       </c>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.3">
@@ -2545,10 +2541,10 @@
         <v>10010034</v>
       </c>
       <c r="B39" s="17" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C39" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D39" s="17">
         <v>35</v>
@@ -2580,8 +2576,8 @@
       <c r="M39" s="17">
         <v>1.3</v>
       </c>
-      <c r="N39" s="17" t="s">
-        <v>31</v>
+      <c r="N39" s="17">
+        <v>0</v>
       </c>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.3">
@@ -2589,10 +2585,10 @@
         <v>10010035</v>
       </c>
       <c r="B40" s="17" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C40" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D40" s="17">
         <v>36</v>
@@ -2624,8 +2620,8 @@
       <c r="M40" s="17">
         <v>1.3</v>
       </c>
-      <c r="N40" s="17" t="s">
-        <v>31</v>
+      <c r="N40" s="17">
+        <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.3">
@@ -2633,10 +2629,10 @@
         <v>10010036</v>
       </c>
       <c r="B41" s="17" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C41" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D41" s="17">
         <v>37</v>
@@ -2668,8 +2664,8 @@
       <c r="M41" s="17">
         <v>1.3</v>
       </c>
-      <c r="N41" s="17" t="s">
-        <v>31</v>
+      <c r="N41" s="17">
+        <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.3">
@@ -2677,10 +2673,10 @@
         <v>10010037</v>
       </c>
       <c r="B42" s="17" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C42" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D42" s="17">
         <v>38</v>
@@ -2712,8 +2708,8 @@
       <c r="M42" s="17">
         <v>1.3</v>
       </c>
-      <c r="N42" s="17" t="s">
-        <v>31</v>
+      <c r="N42" s="17">
+        <v>0</v>
       </c>
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.3">
@@ -2721,10 +2717,10 @@
         <v>10010038</v>
       </c>
       <c r="B43" s="17" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C43" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D43" s="17">
         <v>39</v>
@@ -2756,8 +2752,8 @@
       <c r="M43" s="17">
         <v>1.3</v>
       </c>
-      <c r="N43" s="17" t="s">
-        <v>31</v>
+      <c r="N43" s="17">
+        <v>0</v>
       </c>
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.3">
@@ -2765,10 +2761,10 @@
         <v>10010039</v>
       </c>
       <c r="B44" s="17" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C44" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D44" s="17">
         <v>40</v>
@@ -2800,8 +2796,8 @@
       <c r="M44" s="17">
         <v>1.3</v>
       </c>
-      <c r="N44" s="17" t="s">
-        <v>31</v>
+      <c r="N44" s="17">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>